<commit_message>
序号 4 7 9 10 11 13 15 16 已解
</commit_message>
<xml_diff>
--- a/issue-tracking-2020-feb.xlsx
+++ b/issue-tracking-2020-feb.xlsx
@@ -12,14 +12,14 @@
     <sheet name="2020-2-27" sheetId="3" r:id="rId3"/>
     <sheet name="2020-2-28" sheetId="5" r:id="rId4"/>
     <sheet name="2020-2-29" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId6"/>
+    <sheet name="2020-3-1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37">
   <si>
     <t>序号</t>
   </si>
@@ -63,7 +63,7 @@
     <t>"教师信息管理"-》“教师个人”视图中，当提交过左侧导航栏“学科组”信息后，右侧课程列表视图不正确：打通课程没有按照用分隔符隔开的方式显示，班级没有用“/”分隔符，数据项“平行班级”实际显示的是”打通课程代码“，数据项“是否精品课程”显示的是”平行班级数“。</t>
   </si>
   <si>
-    <t>re-open</t>
+    <t>done</t>
   </si>
   <si>
     <t>"教师信息管理"-》“教师个人”视图中，当左侧导航栏提交过之后，显示的多个班级之间没有用“/”分隔符隔开。</t>
@@ -72,24 +72,21 @@
     <t>"教师信息管理"-》“教师个人”视图中，精品课程的显示：是精品课程显示”精品课程“，不是精品课程显示空（就是什么都没有，不要写none)，其它页面的精品课程也这样。</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>我是不是应该把原来数据库里写在”notes"里的精品课程信息搬到”excellent_course“这个数据项底下去？</t>
   </si>
   <si>
     <t>"教师信息管理"-》“教师个人”视图中，当左侧导航栏选中学科组中的“国际法学”并提交，系统报错。</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>remote</t>
+    <t>course_relate =123</t>
   </si>
   <si>
     <t>系统的日志中，所改动的表格的整行的数据，而不是改动的单元格的数据。这里有没有可能精简？我们可以讨论下，如果精简很麻烦，那可以先放着。</t>
   </si>
   <si>
+    <t>closed</t>
+  </si>
+  <si>
     <t>“课程信息管理”页面中要增加“备注"这一列，”备注“显示”notes“</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>根据上一条，在”历史信息“页面中，要增加”状态“和”备注“两列，显示所有激活非激活的课程，以及显示课程“notes”</t>
   </si>
   <si>
-    <t>备注和激活</t>
-  </si>
-  <si>
     <t>问题：我们现在对于打通课程代码，如果在“课程信息管理页面”中更新了一条课程的相关信息，和它关联的打通课程对应的信息是否会同步更新？如果没有实现这个，我们先记录着，可以之后完善，现在可以和老师说明要求他们手动同步。</t>
   </si>
   <si>
@@ -109,15 +103,6 @@
   </si>
   <si>
     <t>我把LAWS130023的授课老师从“许多奇”改成“陈力”（未申报老师），并且批准微调之后，到“课程信息管理”页面查看，LAWS130023的授课老师显示“陈力”（应该显示“陈力（未申报）”）；而它的打通课程JM630041的授课老师显示的是“陈力（未申报）”（正确）。</t>
-  </si>
-  <si>
-    <t>关于日志，当前只记录course_info的改动，是否可以增加更多的日志，包括：course_adjust_info，teacher_info，users_user</t>
-  </si>
-  <si>
-    <t>“教师信息管理”页面中-》“教务员”-》“微调信息”中，微调求情的状态简化为“已批准”，“已驳回”，“等待审批”</t>
-  </si>
-  <si>
-    <t>已批准，已驳回，等待审批</t>
   </si>
   <si>
     <r>
@@ -127,16 +112,7 @@
         <rFont val="等线"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">关于微调发生过之后，授课老师标注“（已申报）”/“（未申报）”的统一：
-1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t>凡是发生过微调的课程，授课老师一律注明“（已申报）“/”（未申报）“：包括在”课程信息管理“页面中的显示（打通课程也统一）；包括在”教师信息管理“页面中</t>
+      <t>related</t>
     </r>
     <r>
       <rPr>
@@ -145,15 +121,96 @@
         <rFont val="等线"/>
         <charset val="134"/>
       </rPr>
-      <t>"教务员”-》“微调信息”页面中的显示，如果同一课程发生多次（包括第二次及以上）微调，在"微调信息“中，”原授课教师“及”微调教师“都显示"(已申报）”/“（未申报）”（如果是第一次发生微调，只有“微调教师”需要显示“（已申报）”/“（未申报）”）。
-2.排课结束后，点击“锁定”之后，课程信息会复制进历史信息表，发生过微调的课程也携带“（已申报）”/“（未申报）”标识进入历史信息表，这样对历史信息教务员老师可以甄别哪些课程当时是做过人为调整的。</t>
+      <t xml:space="preserve"> to #16</t>
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>关于日志，当前只记录course_info的改动，是否可以增加更多的日志，包括：course_adjust_info，teacher_info</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，users_user</t>
+    </r>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>“教师信息管理”页面中-》“教务员”-》“微调信息”中，微调求情的状态简化为“已批准”，“已驳回”，“等待审批”</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>关于微调发生过之后，授课老师标注“（已申报）”/“（未申报）”的统一：
+1. “课程信息管理”页面中，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>授课老师改成未申报的老师的，一律注明”（未申报）“
+2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>”教师信息管理“-》</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"教务员”-》“微调信息”页面中：“微调教师”要求一律显示“（已申报）”/“（未申报）”标识（现有代码已经实现），”原授课教师“如果是未申报教师的要求显示“（未申报）”标识。
+2.“历史信息”页面，授课教师如果是未申报教师的要求显示“（未申报）”标识。</t>
+    </r>
+  </si>
+  <si>
     <t>如果有”等待审批“的微调还未审批完成，”分配授课教师“步骤四不可以点击”确认完成这一步“，并给出提示”还有微调请求待审批，请完成所有审批。“</t>
   </si>
   <si>
-    <t>”
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">”
 2020-02-28 12:29:11 - 主管老师22222 - [CourseInfo]course_id:laws130023 teacher_final_pick: 陈力
 2020-02-28 12:29:11 - 主管老师22222 - course_relate:JM630041 teacher_final_pick: 陈力(未申报)
 2020-02-29 14:22:53 - 主管老师22222 - [CourseInfo]course_id:927.002.1 teacher_final_pick: 朱丹,张乃根
@@ -162,7 +219,24 @@
 “
 发现这样一段日志，判断是主管老师审批微调之后，在course_info中更新teacher_final_pick时系统做的日志。有几个点：
 1.在更新打通课程的地方没有记录是对哪张表的改动（见第2，4条日志）；
-2.课程代码为927.002.1的打通课程代码为”123“，实际不存在，这种情况实际代码会如何处理？</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2.课程代码为927.002.1的打通课程代码为”123“，实际不存在，这种情况实际代码会如何处理？</t>
+    </r>
+  </si>
+  <si>
+    <t>“分配授课教师”页面-》步骤五-》“锁定排课过程”按键无效。</t>
+  </si>
+  <si>
+    <t>“分配授课教师”页面-》步骤五-》“锁定排课过程”按键建议改名为"锁定排课结果“</t>
   </si>
 </sst>
 </file>
@@ -170,12 +244,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +266,19 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -205,6 +292,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="等线"/>
@@ -214,12 +325,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
@@ -227,9 +346,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,46 +376,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,39 +406,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,7 +439,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -356,181 +619,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,26 +633,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -579,6 +653,41 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -607,37 +716,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -649,10 +738,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -661,153 +750,156 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1181,13 +1273,13 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>43874</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>43886</v>
       </c>
       <c r="G2" t="s">
@@ -1207,13 +1299,13 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>43874</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>43877</v>
       </c>
       <c r="G3" t="s">
@@ -1234,7 +1326,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4" outlineLevelCol="6"/>
@@ -1281,16 +1373,16 @@
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>43882</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>43886</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1301,19 +1393,19 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>43882</v>
       </c>
-      <c r="F3" s="3">
-        <v>43886</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="2">
+        <v>43892</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1327,17 +1419,17 @@
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>43882</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>43886</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" ht="28.5" spans="1:7">
@@ -1348,19 +1440,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>43882</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>43886</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1376,7 +1468,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="6"/>
@@ -1384,10 +1476,10 @@
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="45.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.625" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
     <col min="5" max="5" width="9.875" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="9.25" customWidth="1"/>
+    <col min="6" max="6" width="8.875" customWidth="1"/>
+    <col min="7" max="7" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1420,19 +1512,21 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2">
+        <v>43888</v>
+      </c>
+      <c r="F2" s="2">
+        <v>43892</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="3">
-        <v>43888</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2"/>
     </row>
     <row r="3" ht="42.75" spans="1:6">
       <c r="A3">
@@ -1441,16 +1535,16 @@
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3">
+      <c r="D3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2">
         <v>43888</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" ht="28.5" spans="1:6">
       <c r="A4">
@@ -1459,16 +1553,18 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2">
         <v>43888</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="2">
+        <v>43892</v>
+      </c>
     </row>
     <row r="5" ht="71.25" spans="1:6">
       <c r="A5">
@@ -1477,16 +1573,18 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2">
         <v>43888</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="2">
+        <v>43892</v>
+      </c>
     </row>
     <row r="6" ht="42.75" spans="1:6">
       <c r="A6">
@@ -1495,17 +1593,17 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2">
         <v>43888</v>
       </c>
-      <c r="F6" t="s">
-        <v>26</v>
+      <c r="F6" s="2">
+        <v>43892</v>
       </c>
     </row>
   </sheetData>
@@ -1521,7 +1619,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C17"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="6"/>
@@ -1566,16 +1664,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="3">
+        <v>25</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2">
         <v>43889</v>
       </c>
     </row>
-    <row r="3" ht="85.5" spans="1:5">
+    <row r="3" ht="85.5" spans="1:7">
       <c r="A3">
         <v>13</v>
       </c>
@@ -1583,13 +1681,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="3">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2">
         <v>43889</v>
+      </c>
+      <c r="F3" s="2">
+        <v>43892</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1615,7 +1719,7 @@
     <col min="3" max="3" width="45.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="5.625" customWidth="1"/>
     <col min="5" max="5" width="9.875" customWidth="1"/>
-    <col min="6" max="6" width="25.375" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="9.25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1649,13 +1753,13 @@
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>43890</v>
       </c>
     </row>
@@ -1666,29 +1770,37 @@
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" ht="199.5" spans="1:5">
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2">
+        <v>43870</v>
+      </c>
+      <c r="F3" s="2">
+        <v>43892</v>
+      </c>
+    </row>
+    <row r="4" ht="142.5" spans="1:6">
       <c r="A4">
         <v>16</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="C4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2">
         <v>43890</v>
+      </c>
+      <c r="F4" s="2">
+        <v>43892</v>
       </c>
     </row>
     <row r="5" ht="42.75" spans="1:5">
@@ -1698,13 +1810,13 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="C5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2">
         <v>43890</v>
       </c>
     </row>
@@ -1715,13 +1827,13 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="2">
         <v>43890</v>
       </c>
     </row>
@@ -1735,15 +1847,83 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="45.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.625" customWidth="1"/>
+    <col min="5" max="5" width="9.875" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="9.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" ht="28.5" spans="1:5">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2">
+        <v>43891</v>
+      </c>
+    </row>
+    <row r="3" ht="28.5" spans="1:5">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2">
+        <v>43891</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
all P1 fixed or comments
</commit_message>
<xml_diff>
--- a/issue-tracking-2020-feb.xlsx
+++ b/issue-tracking-2020-feb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050" activeTab="9"/>
+    <workbookView windowWidth="28695" windowHeight="13050" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="2020-2-13" sheetId="1" r:id="rId1"/>
@@ -17,17 +17,20 @@
     <sheet name="2020-3-4" sheetId="9" r:id="rId8"/>
     <sheet name="2020-2-28" sheetId="5" r:id="rId9"/>
     <sheet name="2020-3-8" sheetId="12" r:id="rId10"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId11"/>
+    <sheet name="2020-3-9" sheetId="13" r:id="rId11"/>
+    <sheet name="2020-3-10" sheetId="14" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'2020-3-8'!$A$1:$G$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'2020-3-9'!$A$1:$G$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'2020-3-10'!$A$1:$G$14</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116">
   <si>
     <t>序号</t>
   </si>
@@ -443,18 +446,142 @@
   <si>
     <t>微调那边对更改过的教师和允许教师数会做检查，数目不对不会更改。如果改完允许教师数是符合的，原教师会和新的授课老师难度学时都会更新，但是更新的值是课程的学时/原教师数。这里原教师数根据 #50 做了异常处理</t>
   </si>
+  <si>
+    <t>“历史信息”导出排课结果，导出的workbook里面的那张worksheet的名字必须是“课程信息”，因为之后导入课程的时候，系统会去找那张叫“课程信息”的worksheet。</t>
+  </si>
+  <si>
+    <t>上一学年排课结束之后，要提供一个按钮，可以开始新的一学年排课。需要清掉step_info,course_info,adjust_info,teacher</t>
+  </si>
+  <si>
+    <t>“课程信息管理”页面，“删除改行”按钮失效</t>
+  </si>
+  <si>
+    <t>delete 按钮 关于班级的index出错了</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>“教师信息管理”-》“教师个人”的“申报课程”和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"排课结果“页面中，以及”历史信息“页面中，”班级“信息的中的”-“和”_"连接符（连接学位和年级和班级的连接符）都不要，只保留班级和班级之间的分隔符”/“。</t>
+    </r>
+  </si>
+  <si>
+    <t>”课程信息管理“页面的“编辑课程信息”，弹窗中没有完全加载原有条目中的数据内容。</t>
+  </si>
+  <si>
+    <t>课程导入文件里的状态填写”非激活“的话，导入课程显示是激活的。后台数据库对应数值为”0“</t>
+  </si>
+  <si>
+    <t>历史页面导出的非激活位置不对，我把它放到平行班级之后了</t>
+  </si>
+  <si>
+    <t>”课程信息管理“、”教师信息管理“-》”教师个人“-》”申报课程“页面左侧导航栏中的学位列表和学科组列表要和实际内容一致。现在发现”法律硕士“改名”JM“之后，点击导航栏提交按键后，所有JM的课程无法显示。</t>
+  </si>
+  <si>
+    <t>学位和学期用的是页面的固定值，不是动态获取的。只有学科是。需要做么？</t>
+  </si>
+  <si>
+    <t>加载历史信息似乎把course_info和history_info的数据混起来了。当我把step_info删掉（就是说打算开始新的一学年排课），此时进历史信息，选择2019-2020，系统报错说获取历史信息失败。当我开始2020-2021学年的排课并且导入课程之后，今日历史信息，选择2019-2020，出来的历史课程列表，明显可见打通课程里，所有的被打通的法律硕士的课程都是2020-2021学年新导入的课表里的课程。</t>
+  </si>
+  <si>
+    <t>历史信息导出的打通课程代码，跟当前排课的应该没有任何关系。</t>
+  </si>
+  <si>
+    <t>课程导入文件里“是否精品课程”的值是“精品课程”，因为历史信息的导出就是这个，保持一致比较好。原来用的是“是”，要改成“精品课程”。</t>
+  </si>
+  <si>
+    <t>课程导入时，数据库里的suit_teacher和teacher_ordered应该和excel里的“申报教师”保持一致，而不是“可选教师”，因为历史信息导出的文件里只有”申报教师“，没有”可选教师“（内容是空的）。</t>
+  </si>
+  <si>
+    <t>我把历史导出的可选教师数据跟申报教师写成一致，这样就不需要改导入的代码。</t>
+  </si>
+  <si>
+    <t>课程导入时，把授课教师和备注也带上</t>
+  </si>
+  <si>
+    <t>”课程信息管理“页面上的”非激活课程总数”计数没有把打通课程的去掉。</t>
+  </si>
+  <si>
+    <t>如果有打通课程只算一个？</t>
+  </si>
+  <si>
+    <t>“编辑课程信息”的时候，如果把平行班从“1”改成“2”，确认之后，数据库里的教师数就会*2；并且之后这门课每次用“编辑课程信息”点开再确认，教师数就会*2。关于平行班和教师数，要注意导入，导出和编辑课程信息窗口的统一。</t>
+  </si>
+  <si>
+    <t>步骤二中申报截止时间设定完之后没有自动刷新这个设定按键。</t>
+  </si>
+  <si>
+    <t>教师个人申报课程的弹窗里最下面有个没有名字并且内容为undefined的框。</t>
+  </si>
+  <si>
+    <t>教师个人完成申报的按键会fail</t>
+  </si>
+  <si>
+    <t>需要现场，我本地可以</t>
+  </si>
+  <si>
+    <t>教师个人申报打通课程，申报完了显示申报成功，但是后台数据库并没有写入，所以刷新后就没有了</t>
+  </si>
+  <si>
+    <t>按我的实验结果，有可能是你申报课程的那个用户没有在TeacherInfo的表里面</t>
+  </si>
+  <si>
+    <t>检查申报结果能显示多少信息？我还没开始申报，检查看只有6条。我又试了一个情况应该报5条，实际只报了4条</t>
+  </si>
+  <si>
+    <t>应该全部显示，原判断条件有误。现在应可以了</t>
+  </si>
+  <si>
+    <t>排课异常，log最后如下“2020-03-10 20:12:32 - &lt;STEP 1 Limitation for teacher list&gt;
+2020-03-10 20:12:32 - 课程：CourseInfo object 平行班级情况下，如果申报认识不满足最高要求，但是大于最低要求，会先行安排
+2020-03-10 20:12:32 - 课程：CourseInfo object 平行班级情况下，如果申报认识不满足最高要求，但是大于最低要求，会先行安排
+2020-03-10 20:12:32 - 课程：CourseInfo object 平行班级情况下，如果申报认识不满足最高要求，但是大于最低要求，会先行安排
+2020-03-10 20:12:32 - 排课异常:u''
+”
+而且检查申报情况是没有异常……其实有一门课没有人申报。我把这门课非激活之后还是异常，显示：
+”
+2020-03-10 20:31:14 - &lt;STEP 1 Limitation for teacher list&gt;
+2020-03-10 20:31:14 - 课程：CourseInfo object 平行班级情况下，如果申报认识不满足最高要求，但是大于最低要求，会先行安排
+2020-03-10 20:31:14 - 课程：CourseInfo object 平行班级情况下，如果申报认识不满足最高要求，但是大于最低要求，会先行安排
+2020-03-10 20:31:14 - 课程：CourseInfo object 平行班级情况下，如果申报认识不满足最高要求，但是大于最低要求，会先行安排
+2020-03-10 20:31:14 - 排课异常:u'\u675c\u5b87'
+“</t>
+  </si>
+  <si>
+    <t>这里可能是跟#70的错误有关系</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,66 +604,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -549,9 +617,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -582,6 +649,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -589,8 +663,45 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -614,7 +725,23 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -660,7 +787,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -672,7 +889,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,37 +937,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -726,121 +967,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -857,18 +984,25 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -890,6 +1024,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -906,33 +1055,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -952,17 +1079,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -971,141 +1098,168 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="49" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="49" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="49" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="49" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1114,10 +1268,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1129,29 +1286,29 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
     <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
@@ -1201,6 +1358,7 @@
     <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="常规 2" xfId="49"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1495,7 +1653,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -1507,7 +1665,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1518,16 +1676,16 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="13">
         <v>43874</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="13">
         <v>43886</v>
       </c>
       <c r="G2" t="s">
@@ -1547,13 +1705,13 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="13">
         <v>43874</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="13">
         <v>43877</v>
       </c>
       <c r="G3" t="s">
@@ -1571,15 +1729,15 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="5.25" customWidth="1"/>
     <col min="2" max="2" width="7.125" customWidth="1"/>
-    <col min="3" max="3" width="54.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="54.625" style="10" customWidth="1"/>
     <col min="4" max="4" width="8.375" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
@@ -1593,7 +1751,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -1605,7 +1763,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1616,16 +1774,16 @@
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="13">
         <v>43898</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="13">
         <v>43899</v>
       </c>
       <c r="G2" t="s">
@@ -1639,16 +1797,16 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="D3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="13">
         <v>43898</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="13">
         <v>43899</v>
       </c>
     </row>
@@ -1659,19 +1817,19 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="13">
         <v>43898</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="13">
         <v>43899</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1682,16 +1840,16 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="13">
         <v>43898</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="13">
         <v>43899</v>
       </c>
     </row>
@@ -1702,16 +1860,16 @@
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="13">
         <v>43898</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="13">
         <v>43899</v>
       </c>
     </row>
@@ -1722,16 +1880,16 @@
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="13">
         <v>43898</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" ht="28.5" spans="1:6">
       <c r="A8">
@@ -1740,16 +1898,16 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="D8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="13">
         <v>43898</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="13">
         <v>43899</v>
       </c>
     </row>
@@ -1760,65 +1918,65 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="13">
         <v>43898</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="13">
         <v>43899</v>
       </c>
       <c r="G9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" s="1" customFormat="1" ht="141.75" hidden="1" spans="1:7">
-      <c r="A10" s="1">
+    <row r="10" s="8" customFormat="1" ht="141.75" hidden="1" spans="1:7">
+      <c r="A10" s="8">
         <v>16</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="8">
         <v>2</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="17">
         <v>43890</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="17">
         <v>43892</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" ht="71.25" spans="1:7">
-      <c r="A11" s="1">
+    <row r="11" s="9" customFormat="1" ht="71.25" spans="1:7">
+      <c r="A11" s="9">
         <v>33</v>
       </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="8">
+      <c r="D11" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="20">
         <v>43897</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="20">
         <v>43899</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="18" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1829,13 +1987,13 @@
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="13">
         <v>43898</v>
       </c>
     </row>
@@ -1846,13 +2004,13 @@
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="13">
         <v>43898</v>
       </c>
     </row>
@@ -1863,13 +2021,13 @@
       <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="13">
         <v>43898</v>
       </c>
     </row>
@@ -1880,13 +2038,13 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="13">
         <v>43898</v>
       </c>
     </row>
@@ -1897,50 +2055,50 @@
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="13">
         <v>43898</v>
       </c>
     </row>
-    <row r="17" ht="28.5" spans="1:7">
+    <row r="17" ht="28.5" hidden="1" spans="1:7">
       <c r="A17">
         <v>48</v>
       </c>
       <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="13">
         <v>43898</v>
       </c>
       <c r="G17" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" ht="28.5" spans="1:7">
+    <row r="18" ht="28.5" hidden="1" spans="1:7">
       <c r="A18">
         <v>49</v>
       </c>
       <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="13">
         <v>43898</v>
       </c>
       <c r="G18" t="s">
@@ -1954,13 +2112,13 @@
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="13">
         <v>43898</v>
       </c>
     </row>
@@ -1971,13 +2129,13 @@
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="13">
         <v>43898</v>
       </c>
       <c r="G20" t="s">
@@ -1991,13 +2149,13 @@
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="13">
         <v>43898</v>
       </c>
       <c r="G21" t="s">
@@ -2021,15 +2179,519 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="5.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7" style="1" customWidth="1"/>
+    <col min="3" max="3" width="54.375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="56.625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" ht="42.75" spans="1:6">
+      <c r="A2" s="1">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="4">
+        <v>43898</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" ht="28.5" spans="1:6">
+      <c r="A3" s="1">
+        <v>54</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="4">
+        <v>43898</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4">
+        <v>43898</v>
+      </c>
+      <c r="F4" s="4">
+        <v>43900</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" ht="57" spans="1:6">
+      <c r="A5" s="1">
+        <v>56</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="4">
+        <v>43898</v>
+      </c>
+      <c r="F5" s="4">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="6" ht="28.5" spans="1:6">
+      <c r="A6" s="1">
+        <v>57</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4">
+        <v>43898</v>
+      </c>
+      <c r="F6" s="4">
+        <v>43899</v>
+      </c>
+    </row>
+    <row r="7" ht="28.5" spans="1:7">
+      <c r="A7" s="1">
+        <v>58</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="4">
+        <v>43898</v>
+      </c>
+      <c r="F7" s="4">
+        <v>43900</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="5:5">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="5:5">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" s="3" customFormat="1" spans="3:7">
+      <c r="C10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" s="3" customFormat="1" spans="3:7">
+      <c r="C11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="5:5">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="5:5">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="5:5">
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="5:5">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="5:5">
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="5:5">
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="5:5">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="5:5">
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="5:5">
+      <c r="E21" s="4"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G7"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="5.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7" style="1" customWidth="1"/>
+    <col min="3" max="3" width="54.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="71.25" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" ht="57" spans="1:7">
+      <c r="A2" s="1">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="4">
+        <v>43900</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" ht="99.75" spans="1:7">
+      <c r="A3" s="1">
+        <v>61</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="4">
+        <v>43900</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" ht="42.75" spans="1:6">
+      <c r="A4" s="1">
+        <v>62</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4">
+        <v>43900</v>
+      </c>
+      <c r="F4" s="4">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="5" ht="42.75" spans="1:7">
+      <c r="A5" s="1">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="4">
+        <v>43900</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" hidden="1" spans="1:5">
+      <c r="A6" s="1">
+        <v>64</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="4">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="7" ht="28.5" spans="1:7">
+      <c r="A7" s="1">
+        <v>65</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="4">
+        <v>43900</v>
+      </c>
+      <c r="F7" s="4">
+        <v>43900</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" ht="57" spans="1:5">
+      <c r="A8" s="1">
+        <v>66</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="4">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>67</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="4">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="10" ht="28.5" hidden="1" spans="3:3">
+      <c r="C10" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1">
+        <v>68</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="4">
+        <v>43900</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" ht="28.5" spans="1:7">
+      <c r="A12" s="1">
+        <v>69</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="4">
+        <v>43900</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" ht="28.5" spans="1:7">
+      <c r="A13" s="1">
+        <v>70</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="4">
+        <v>43900</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" ht="399" spans="1:7">
+      <c r="A14" s="1">
+        <v>71</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="4">
+        <v>43900</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G14">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="equal" val="1"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2049,7 +2711,7 @@
   <cols>
     <col min="1" max="1" width="5.25" customWidth="1"/>
     <col min="2" max="2" width="7.125" customWidth="1"/>
-    <col min="3" max="3" width="50.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50.25" style="10" customWidth="1"/>
     <col min="4" max="4" width="8.375" customWidth="1"/>
     <col min="5" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="54.375" customWidth="1"/>
@@ -2063,7 +2725,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -2075,7 +2737,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2086,19 +2748,19 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="13">
         <v>43882</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="13">
         <v>43886</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2109,19 +2771,19 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="13">
         <v>43882</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="13">
         <v>43892</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="11" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2132,16 +2794,16 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="13">
         <v>43882</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="13">
         <v>43886</v>
       </c>
       <c r="G4" t="s">
@@ -2155,16 +2817,16 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="13">
         <v>43882</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="13">
         <v>43886</v>
       </c>
       <c r="G5" t="s">
@@ -2193,7 +2855,7 @@
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="45.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.625" style="10" customWidth="1"/>
     <col min="4" max="4" width="6.625" customWidth="1"/>
     <col min="5" max="5" width="9.875" customWidth="1"/>
     <col min="6" max="6" width="8.875" customWidth="1"/>
@@ -2207,7 +2869,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -2219,7 +2881,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2230,19 +2892,19 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="13">
         <v>43888</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="13">
         <v>43892</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="14" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2253,16 +2915,16 @@
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="13">
         <v>43888</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" ht="28.5" spans="1:6">
       <c r="A4">
@@ -2271,16 +2933,16 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="13">
         <v>43888</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="13">
         <v>43892</v>
       </c>
     </row>
@@ -2291,16 +2953,16 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="13">
         <v>43888</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="13">
         <v>43892</v>
       </c>
     </row>
@@ -2311,16 +2973,16 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="13">
         <v>43888</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="13">
         <v>43892</v>
       </c>
     </row>
@@ -2346,7 +3008,7 @@
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="45.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.625" style="10" customWidth="1"/>
     <col min="4" max="4" width="5.625" customWidth="1"/>
     <col min="5" max="5" width="9.875" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
@@ -2360,7 +3022,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -2372,7 +3034,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2383,16 +3045,16 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="13">
         <v>43891</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="13">
         <v>43893</v>
       </c>
       <c r="G2" t="s">
@@ -2406,16 +3068,16 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="13">
         <v>43891</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="13">
         <v>43893</v>
       </c>
     </row>
@@ -2441,7 +3103,7 @@
   <cols>
     <col min="1" max="1" width="5.25" customWidth="1"/>
     <col min="2" max="2" width="7.125" customWidth="1"/>
-    <col min="3" max="3" width="50.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50.5" style="10" customWidth="1"/>
     <col min="4" max="4" width="8.5" customWidth="1"/>
     <col min="5" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="10.125" customWidth="1"/>
@@ -2454,7 +3116,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -2466,7 +3128,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2477,16 +3139,16 @@
       <c r="B2">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="13">
         <v>43896</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="13">
         <v>43898</v>
       </c>
       <c r="G2" t="s">
@@ -2500,55 +3162,55 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="13">
         <v>43896</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="13">
         <v>43898</v>
       </c>
     </row>
-    <row r="4" s="10" customFormat="1" ht="185.25" spans="1:6">
-      <c r="A4" s="10">
+    <row r="4" s="9" customFormat="1" ht="185.25" spans="1:6">
+      <c r="A4" s="9">
         <v>29</v>
       </c>
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="20">
         <v>43896</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="20">
         <v>43898</v>
       </c>
     </row>
     <row r="5" spans="3:6">
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="3:6">
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="3:5">
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2572,7 +3234,7 @@
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
     <col min="2" max="2" width="2.5" customWidth="1"/>
-    <col min="3" max="3" width="49.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="49.125" style="10" customWidth="1"/>
     <col min="4" max="4" width="8.5" customWidth="1"/>
     <col min="5" max="5" width="10.125" customWidth="1"/>
     <col min="6" max="6" width="9.125" customWidth="1"/>
@@ -2586,7 +3248,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -2598,7 +3260,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2609,16 +3271,16 @@
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="13">
         <v>43890</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="13">
         <v>43893</v>
       </c>
     </row>
@@ -2629,16 +3291,16 @@
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="13">
         <v>43870</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="13">
         <v>43892</v>
       </c>
     </row>
@@ -2649,16 +3311,16 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="13">
         <v>43890</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="13">
         <v>43893</v>
       </c>
     </row>
@@ -2669,16 +3331,16 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="13">
         <v>43890</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="13">
         <v>43893</v>
       </c>
     </row>
@@ -2704,7 +3366,7 @@
   <cols>
     <col min="1" max="1" width="5.25" customWidth="1"/>
     <col min="2" max="2" width="7.125" customWidth="1"/>
-    <col min="3" max="3" width="50.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50.5" style="10" customWidth="1"/>
     <col min="4" max="4" width="8.5" customWidth="1"/>
     <col min="5" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="37.5" customWidth="1"/>
@@ -2717,7 +3379,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -2729,7 +3391,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2740,16 +3402,16 @@
       <c r="B2">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="13">
         <v>43897</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="13">
         <v>43898</v>
       </c>
     </row>
@@ -2760,16 +3422,16 @@
       <c r="B3">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="13">
         <v>43897</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="13">
         <v>43898</v>
       </c>
     </row>
@@ -2780,16 +3442,16 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="13">
         <v>43897</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="13">
         <v>43898</v>
       </c>
     </row>
@@ -2800,16 +3462,16 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="13">
         <v>43897</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="13">
         <v>43898</v>
       </c>
     </row>
@@ -2835,7 +3497,7 @@
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="45.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.625" style="10" customWidth="1"/>
     <col min="4" max="4" width="5.625" customWidth="1"/>
     <col min="5" max="5" width="8.875" customWidth="1"/>
     <col min="6" max="6" width="32.125" customWidth="1"/>
@@ -2849,7 +3511,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -2861,7 +3523,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2872,16 +3534,16 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="13">
         <v>43894</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="13">
         <v>43895</v>
       </c>
       <c r="G2" t="s">
@@ -2895,16 +3557,16 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="13">
         <v>43894</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="13">
         <v>43895</v>
       </c>
     </row>
@@ -2915,42 +3577,42 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="13">
         <v>43894</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="13">
         <v>43895</v>
       </c>
       <c r="G4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" s="10" customFormat="1" ht="71.25" spans="1:7">
-      <c r="A5" s="10">
+    <row r="5" s="9" customFormat="1" ht="71.25" spans="1:7">
+      <c r="A5" s="9">
         <v>24</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>5</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="20">
         <v>43894</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="20">
         <v>43895</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="18" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2961,16 +3623,16 @@
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="13">
         <v>43894</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="13">
         <v>43895</v>
       </c>
       <c r="G6" t="s">
@@ -2984,13 +3646,13 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="13">
         <v>43894</v>
       </c>
       <c r="G7" t="s">
@@ -3012,14 +3674,14 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="45.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.625" style="10" customWidth="1"/>
     <col min="4" max="4" width="5.625" customWidth="1"/>
     <col min="5" max="5" width="9.875" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
@@ -3033,7 +3695,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -3045,7 +3707,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3056,13 +3718,13 @@
       <c r="B2">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="13">
         <v>43889</v>
       </c>
       <c r="G2" t="s">
@@ -3076,19 +3738,19 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="10" t="s">
         <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="13">
         <v>43889</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="13">
         <v>43892</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="14" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>